<commit_message>
Added length to analysis
</commit_message>
<xml_diff>
--- a/Test/MSA_info.xlsx
+++ b/Test/MSA_info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
   <si>
     <t xml:space="preserve">Dataset 1</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original</t>
   </si>
   <si>
     <t xml:space="preserve">Remained</t>
@@ -208,7 +211,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -235,9 +238,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>444240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -251,7 +254,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7776720" cy="1279800"/>
+          <a:ext cx="7782120" cy="1279440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -272,9 +275,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -288,7 +291,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1360440"/>
-          <a:ext cx="6521400" cy="4224600"/>
+          <a:ext cx="6526080" cy="4224240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>491040</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7112160" y="691560"/>
+          <a:ext cx="7239600" cy="2466720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -314,13 +354,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>760320</xdr:colOff>
+      <xdr:colOff>759960</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 3" descr=""/>
+        <xdr:cNvPr id="3" name="Image 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -330,7 +370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="286200" y="331200"/>
-          <a:ext cx="7806240" cy="1490400"/>
+          <a:ext cx="7811640" cy="1490040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -344,20 +384,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>254880</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>489600</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>429480</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 6" descr=""/>
+        <xdr:cNvPr id="4" name="Image 6" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -366,8 +406,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1069560" y="1995840"/>
-          <a:ext cx="13269960" cy="4313880"/>
+          <a:off x="0" y="678960"/>
+          <a:ext cx="10213560" cy="3317400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -393,13 +433,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>229320</xdr:colOff>
+      <xdr:colOff>228960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 1" descr=""/>
+        <xdr:cNvPr id="5" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -409,7 +449,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1456200"/>
-          <a:ext cx="6746760" cy="859320"/>
+          <a:ext cx="6751440" cy="858960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -430,13 +470,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>766440</xdr:colOff>
+      <xdr:colOff>766080</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4" descr=""/>
+        <xdr:cNvPr id="6" name="Image 4" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -446,7 +486,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7283880" cy="1681560"/>
+          <a:ext cx="7288560" cy="1681200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -467,13 +507,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>745560</xdr:colOff>
+      <xdr:colOff>745200</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 7" descr=""/>
+        <xdr:cNvPr id="7" name="Image 7" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -482,8 +522,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2866320" y="969120"/>
-          <a:ext cx="7655400" cy="3604320"/>
+          <a:off x="2868120" y="969120"/>
+          <a:ext cx="7661160" cy="3603960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -509,7 +549,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.43"/>
@@ -846,11 +886,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -873,10 +913,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -927,7 +967,7 @@
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,13 +992,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.4"/>
@@ -1053,10 +1093,13 @@
       <c r="G7" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="H7" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>102</v>
@@ -1071,6 +1114,9 @@
         <v>97</v>
       </c>
       <c r="G8" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>102</v>
       </c>
     </row>
@@ -1091,6 +1137,9 @@
       <c r="G9" s="0" t="n">
         <v>1068</v>
       </c>
+      <c r="H9" s="0" t="n">
+        <v>1068</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2"/>
@@ -1109,6 +1158,9 @@
       <c r="G10" s="0" t="n">
         <v>2034</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>1068</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
@@ -1126,10 +1178,13 @@
       <c r="G12" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="H12" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>102</v>
@@ -1145,6 +1200,9 @@
       </c>
       <c r="G13" s="0" t="n">
         <v>98.78</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>46.73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,6 +1222,9 @@
       <c r="G14" s="0" t="n">
         <v>96.32</v>
       </c>
+      <c r="H14" s="0" t="n">
+        <v>10.5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2"/>
@@ -1182,6 +1243,9 @@
       <c r="G15" s="0" t="n">
         <v>93.3</v>
       </c>
+      <c r="H15" s="0" t="n">
+        <v>7.24</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
@@ -1199,10 +1263,13 @@
       <c r="G17" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="H17" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>102</v>
@@ -1218,6 +1285,9 @@
       </c>
       <c r="G18" s="0" t="n">
         <v>0.21</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.09</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,6 +1307,9 @@
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2"/>
@@ -1255,6 +1328,9 @@
       <c r="G20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
@@ -1272,10 +1348,13 @@
       <c r="G22" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="H22" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>102</v>
@@ -1291,6 +1370,9 @@
       </c>
       <c r="G23" s="0" t="n">
         <v>-349.82</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>-456.99</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,6 +1392,9 @@
       <c r="G24" s="0" t="n">
         <v>-815.43</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <v>-1542.62</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2"/>
@@ -1328,14 +1413,103 @@
       <c r="G25" s="0" t="n">
         <v>-2066.42</v>
       </c>
+      <c r="H25" s="0" t="n">
+        <v>-3126.18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1002</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1002</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1515</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>976</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2"/>
+      <c r="C29" s="0" t="n">
+        <v>1068</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>1668</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1668</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>11443</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1667</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>15987</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2"/>
+      <c r="C30" s="0" t="n">
+        <v>2034</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>2334</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>2334</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>2333</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>32453</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>